<commit_message>
Add markdown and math support for bot messages
Enhanced bot message rendering to support markdown formatting and LaTeX math expressions by introducing a markdown parser in script.js and corresponding CSS styles. Removed most console logging for cleaner production output. Updated README with acknowledgments and performed plugin file maintenance.
</commit_message>
<xml_diff>
--- a/extras/test-form/plugin_test_form_text.xlsx
+++ b/extras/test-form/plugin_test_form_text.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10921"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitoworks/Downloads/GitHub/chatbot-demo/extras/test-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672F90DE-349C-354E-B88C-0B35DE7C484F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60FE504-2657-C746-A21F-C013AC20C423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41120" yWindow="3220" windowWidth="51200" windowHeight="28300" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41120" yWindow="2720" windowWidth="51200" windowHeight="28800" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="397">
   <si>
     <t>type</t>
   </si>
@@ -2594,9 +2594,6 @@
     <t>read only</t>
   </si>
   <si>
-    <t>hint:عربى</t>
-  </si>
-  <si>
     <t>constraint message:عربى</t>
   </si>
   <si>
@@ -2639,12 +2636,6 @@
     <t>Get your API key from https://platform.openai.com/api-keys</t>
   </si>
   <si>
-    <t>Chatbot Demo Test Form</t>
-  </si>
-  <si>
-    <t>chatbot_demo_test</t>
-  </si>
-  <si>
     <t>chat_test1</t>
   </si>
   <si>
@@ -2654,24 +2645,6 @@
     <t>chat_test3</t>
   </si>
   <si>
-    <t>custom-chatbot(api-key=${api_key}, system_prompt='You are a helpful customer service representative for a pizza restaurant. Be friendly and help customers with orders, hours, and basic questions. Keep responses short and conversational.',
-    suggested-prompts='What are your hours?|Menu options|Place an order|Store location',
-    timeout=300)</t>
-  </si>
-  <si>
-    <t>custom-chatbot(api-key=${api_key},system_prompt='You are conducting a job interview for a data collector position. Ask typical interview questions one at a time. Be professional but encouraging. After 5-6 questions, provide brief feedback and end with Thank you for your time. END_CONVERSATION',
-    case_data='The candidate is applying for: data collection at SurveyCTO',
-    suggested-prompts='Tell me about yourself|Why this role?|My experience|Ask a question',
-    timeout=900,
-    end-message='Interview complete. Good luck!')</t>
-  </si>
-  <si>
-    <t>custom-chatbot(api-key=${api_key},    system_prompt='You are a math tutor helping a student with basic algebra. Ask them what they want to work on, then provide step-by-step help. Use simple language and encourage them.',
-    conversation-starter="Ask the student what math topic they'd like help with today",
-    suggested-prompts="Help with equations|Explain fractions|Practice problems|I'm stuck",
-    end-message='Great job today! Keep practicing!')</t>
-  </si>
-  <si>
     <t>Basic Customer Service Bot</t>
   </si>
   <si>
@@ -2679,6 +2652,30 @@
   </si>
   <si>
     <t>Job Interview Practice</t>
+  </si>
+  <si>
+    <t>chat_test4</t>
+  </si>
+  <si>
+    <t>Advanced Demo with End Codes</t>
+  </si>
+  <si>
+    <t>LLM Conversations Field plug-in Test Form</t>
+  </si>
+  <si>
+    <t>llm_conversations_test_form</t>
+  </si>
+  <si>
+    <t>custom-llm-conversations(api-key=${api_key}, system_prompt='You are a helpful customer service representative for a pizza restaurant. Be friendly and help customers with orders, hours, and basic questions. Keep responses short and conversational.', suggested-prompts='What are your hours?|Menu options|Place an order|Store location', timeout=300)</t>
+  </si>
+  <si>
+    <t>custom-llm-conversations(api-key=${api_key}, system_prompt='You are a math tutor helping a student with basic algebra. Ask them what they want to work on, then provide step-by-step help. Use simple language and encourage them.', conversation-starter='Ask the student what math topic they would like help with today', suggested-prompts='Help with equations|Explain fractions|Practice problems|I am stuck', end-message='Great job today! Keep practicing!')</t>
+  </si>
+  <si>
+    <t>custom-llm-conversations(api-key=${api_key}, system_prompt='You are conducting a job interview for a data collector position. Ask typical interview questions one at a time. Be professional but encouraging. After 5-6 questions, provide brief feedback and end with: Thank you for your time. END_CONVERSATION', case_data='The candidate is applying for: data collection at SurveyCTO', suggested-prompts='Tell me about yourself|Why this role?|My experience|Ask a question', timeout=900, end-message='Interview complete. Good luck!')</t>
+  </si>
+  <si>
+    <t>custom-llm-conversations(api-key=${api_key}, system_prompt='You are a helpful assistant. Have a brief conversation, then when the user asks to end or after 3-4 exchanges, say goodbye and include the code 5j3k to end the conversation.', suggested-prompts='Hello|Tell me a joke|Help with something|End conversation', clear-button-label='Clear Chat', complete-button-label='Finish')</t>
   </si>
 </sst>
 </file>
@@ -3374,6 +3371,64 @@
   <dxfs count="203">
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
@@ -3383,6 +3438,50 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
@@ -3425,6 +3524,39 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="6" tint="0.59999389629810485"/>
@@ -3433,6 +3565,14 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
@@ -3449,6 +3589,14 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3462,6 +3610,350 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFDCC97A"/>
@@ -3470,96 +3962,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFE4E300"/>
@@ -3568,61 +3970,15 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3630,365 +3986,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4036,6 +4033,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
@@ -4078,19 +4089,102 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4099,6 +4193,302 @@
         <color auto="1"/>
       </font>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.249977111117893"/>
@@ -4106,9 +4496,195 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4121,6 +4697,121 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -4130,13 +4821,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
@@ -4153,14 +4837,22 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4175,7 +4867,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4183,94 +4882,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor rgb="FF9E004F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4286,192 +4898,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
+          <bgColor rgb="FFFBFB00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4482,439 +4911,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5333,11 +5330,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF16"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5346,31 +5343,30 @@
     <col min="2" max="2" width="40.5" style="9" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="30.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="23" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23" style="11" customWidth="1"/>
-    <col min="6" max="6" width="46" style="9" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.33203125" style="9" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.1640625" style="9" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.33203125" style="9" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18" style="9" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.5" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15" style="9" customWidth="1" collapsed="1"/>
-    <col min="19" max="20" width="48" style="9" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="26" width="11" style="2" collapsed="1"/>
-    <col min="27" max="30" width="11" style="2"/>
-    <col min="31" max="31" width="11" style="2" collapsed="1"/>
-    <col min="32" max="32" width="11" style="2"/>
+    <col min="5" max="5" width="46" style="9" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="82.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17" style="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.33203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18" style="9" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.5" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15" style="9" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="48" style="9" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="25" width="11" style="2" collapsed="1"/>
+    <col min="26" max="29" width="11" style="2"/>
+    <col min="30" max="30" width="11" style="2" collapsed="1"/>
+    <col min="31" max="32" width="11" style="2"/>
     <col min="33" max="16384" width="11" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5383,47 +5379,47 @@
       <c r="D1" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="O1" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>368</v>
-      </c>
       <c r="Q1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>372</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>373</v>
@@ -5432,315 +5428,326 @@
         <v>374</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="V1" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="V1" t="s">
+        <v>33</v>
+      </c>
       <c r="W1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X1" t="s">
-        <v>34</v>
+        <v>284</v>
       </c>
       <c r="Y1" t="s">
-        <v>284</v>
-      </c>
-      <c r="Z1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="J2" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="K2" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L2" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="X3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="J4" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="K4" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L4" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="X4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="J5" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="K5" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="X5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>358</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L6" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="X6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="J7" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="K7" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L7" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="X7" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>296</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>296</v>
       </c>
+      <c r="J8" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="K8" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L8" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="X8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>295</v>
       </c>
+      <c r="J9" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="K9" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L9" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="P9" t="s">
         <v>293</v>
       </c>
-      <c r="Y9" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="X9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>292</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>292</v>
       </c>
+      <c r="J10" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="K10" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="X10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="J11" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="Y10" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="K11" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="L11" s="11" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C12" t="s">
         <v>378</v>
       </c>
-      <c r="C12" t="s">
-        <v>379</v>
-      </c>
       <c r="D12" t="s">
-        <v>382</v>
-      </c>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D13" t="s">
-        <v>383</v>
-      </c>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:25" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>87</v>
       </c>
       <c r="B14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C14" t="s">
         <v>386</v>
       </c>
-      <c r="C14" t="s">
-        <v>392</v>
-      </c>
       <c r="D14"/>
-      <c r="G14" s="20" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="204" x14ac:dyDescent="0.2">
+      <c r="F14" s="20" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>87</v>
       </c>
       <c r="B15" t="s">
+        <v>384</v>
+      </c>
+      <c r="C15" t="s">
         <v>387</v>
       </c>
-      <c r="C15" t="s">
-        <v>393</v>
-      </c>
       <c r="D15"/>
-      <c r="G15" s="20" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="255" x14ac:dyDescent="0.2">
+      <c r="F15" s="20" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="102" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>87</v>
       </c>
       <c r="B16" t="s">
+        <v>385</v>
+      </c>
+      <c r="C16" t="s">
         <v>388</v>
       </c>
-      <c r="C16" t="s">
-        <v>394</v>
-      </c>
       <c r="D16"/>
-      <c r="G16" s="20" t="s">
+      <c r="F16" s="20" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>390</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A12:B16 B17:B1048576">
-    <cfRule type="expression" dxfId="202" priority="1430" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="1422" stopIfTrue="1">
+      <formula>$A12="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="201" priority="1430" stopIfTrue="1">
       <formula>OR($A12="calculate", $A12="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="1422" stopIfTrue="1">
-      <formula>$A12="comments"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C11 F1:V1048576">
+  <conditionalFormatting sqref="A1:C11 E1:U1048576">
     <cfRule type="expression" dxfId="200" priority="881" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="2155" stopIfTrue="1">
-      <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="198" priority="2152" stopIfTrue="1">
-      <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="197" priority="2150" stopIfTrue="1">
-      <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="196" priority="2148" stopIfTrue="1">
-      <formula>$A1="barcode"</formula>
+    <cfRule type="expression" dxfId="199" priority="2136" stopIfTrue="1">
+      <formula>OR($A1="audio", $A1="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="198" priority="2138" stopIfTrue="1">
+      <formula>$A1="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="197" priority="2142" stopIfTrue="1">
+      <formula>OR($A1="date", $A1="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="196" priority="2144" stopIfTrue="1">
+      <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="195" priority="2146" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="2144" stopIfTrue="1">
-      <formula>OR($A1="calculate", $A1="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="193" priority="2142" stopIfTrue="1">
-      <formula>OR($A1="date", $A1="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="192" priority="2138" stopIfTrue="1">
-      <formula>$A1="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="191" priority="2136" stopIfTrue="1">
-      <formula>OR($A1="audio", $A1="video")</formula>
+    <cfRule type="expression" dxfId="194" priority="2148" stopIfTrue="1">
+      <formula>$A1="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="193" priority="2150" stopIfTrue="1">
+      <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="192" priority="2152" stopIfTrue="1">
+      <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="191" priority="2155" stopIfTrue="1">
+      <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576 F1:V1048576">
-    <cfRule type="expression" dxfId="190" priority="2172" stopIfTrue="1">
-      <formula>$A1="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="189" priority="2171" stopIfTrue="1">
-      <formula>$A1="text"</formula>
+  <conditionalFormatting sqref="A1:C1048576 E1:U1048576">
+    <cfRule type="expression" dxfId="190" priority="2162" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="189" priority="2167" stopIfTrue="1">
+      <formula>$A1="decimal"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="188" priority="2169" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="2167" stopIfTrue="1">
-      <formula>$A1="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="186" priority="2162" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
+    <cfRule type="expression" dxfId="187" priority="2171" stopIfTrue="1">
+      <formula>$A1="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="186" priority="2172" stopIfTrue="1">
+      <formula>$A1="end repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="185" priority="2174" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
@@ -5752,45 +5759,45 @@
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:C16 B17:C1048576 G1:G1048576">
+  <conditionalFormatting sqref="A12:C16 B17:C1048576 F1:F1048576">
     <cfRule type="expression" dxfId="182" priority="1811" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:C16 B17:C1048576 K1:K1048576">
+  <conditionalFormatting sqref="A12:C16 B17:C1048576 J1:J1048576">
     <cfRule type="expression" dxfId="181" priority="1835" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:C16 B17:C1048576">
-    <cfRule type="expression" dxfId="180" priority="1436" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="1424" stopIfTrue="1">
+      <formula>OR($A12="audio", $A12="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="179" priority="1432" stopIfTrue="1">
+      <formula>$A12="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="178" priority="1434" stopIfTrue="1">
+      <formula>$A12="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="177" priority="1436" stopIfTrue="1">
       <formula>OR($A12="geopoint", $A12="geoshape", $A12="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="179" priority="1434" stopIfTrue="1">
-      <formula>$A12="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="178" priority="1432" stopIfTrue="1">
-      <formula>$A12="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="177" priority="1424" stopIfTrue="1">
-      <formula>OR($A12="audio", $A12="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:D1048576">
-    <cfRule type="expression" dxfId="176" priority="1324" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="1316" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="175" priority="1318" stopIfTrue="1">
+      <formula>$A12="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="174" priority="1320" stopIfTrue="1">
+      <formula>OR($A12="audio", $A12="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="173" priority="1322" stopIfTrue="1">
+      <formula>$A12="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="1324" stopIfTrue="1">
       <formula>OR($A12="date", $A12="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="175" priority="1316" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="174" priority="1318" stopIfTrue="1">
-      <formula>$A12="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="173" priority="1320" stopIfTrue="1">
-      <formula>OR($A12="audio", $A12="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="172" priority="1322" stopIfTrue="1">
-      <formula>$A12="image"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="171" priority="1326" stopIfTrue="1">
       <formula>OR($A12="calculate", $A12="calculate_here")</formula>
@@ -5819,7 +5826,7 @@
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 G1:G1048576 A12:A16">
+  <conditionalFormatting sqref="B1:B1048576 F1:F1048576 A12:A16">
     <cfRule type="expression" dxfId="163" priority="811" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
@@ -5828,42 +5835,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C11">
-    <cfRule type="expression" dxfId="161" priority="2141" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="2135" stopIfTrue="1">
+      <formula>OR($A1="audio", $A1="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="2137" stopIfTrue="1">
+      <formula>$A1="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="159" priority="2141" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="2135" stopIfTrue="1">
-      <formula>OR($A1="audio", $A1="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="159" priority="2145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="2145" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="2147" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="2147" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="2149" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="2149" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="2173" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="2173" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="2176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="2176" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="2137" stopIfTrue="1">
-      <formula>$A1="image"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 G1:G1048576 A12:B16 D12:D1048576">
+  <conditionalFormatting sqref="B1:C1048576 F1:F1048576 A12:B16 D12:D1048576">
     <cfRule type="expression" dxfId="153" priority="2170" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 G1:G1048576 A12:B16">
+  <conditionalFormatting sqref="B1:C1048576 F1:F1048576 A12:B16">
     <cfRule type="expression" dxfId="152" priority="2161" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 H1:J1048576 A12:B16">
+  <conditionalFormatting sqref="B1:C1048576 G1:I1048576 A12:B16">
     <cfRule type="expression" dxfId="151" priority="2166" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
@@ -5872,211 +5879,211 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C16">
-    <cfRule type="expression" dxfId="149" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="1" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="148" priority="2" stopIfTrue="1">
+      <formula>$A12="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="147" priority="3" stopIfTrue="1">
+      <formula>OR($A12="audio", $A12="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="4" stopIfTrue="1">
+      <formula>$A12="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="5" stopIfTrue="1">
+      <formula>OR($A12="date", $A12="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="6" stopIfTrue="1">
+      <formula>OR($A12="calculate", $A12="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="7" stopIfTrue="1">
       <formula>$A12="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="8" stopIfTrue="1">
+      <formula>$A12="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="9" stopIfTrue="1">
+      <formula>OR($A12="geopoint", $A12="geoshape", $A12="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="10" stopIfTrue="1">
+      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="11" stopIfTrue="1">
+      <formula>OR($A12="username", $A12="phonenumber", $A12="start", $A12="end", $A12="deviceid", $A12="subscriberid", $A12="simserial", $A12="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="12" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="137" priority="13" stopIfTrue="1">
+      <formula>$A12="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="14" stopIfTrue="1">
+      <formula>$A12="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="135" priority="15" stopIfTrue="1">
+      <formula>$A12="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="16" stopIfTrue="1">
+      <formula>$A12="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="17" stopIfTrue="1">
+      <formula>$A12="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="18" stopIfTrue="1">
+      <formula>$A12="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="19" stopIfTrue="1">
+      <formula>$A12="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="20" stopIfTrue="1">
+      <formula>$A12="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="129" priority="21" stopIfTrue="1">
+      <formula>$A12="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="22" stopIfTrue="1">
+      <formula>$A12="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="127" priority="23" stopIfTrue="1">
+      <formula>$A12="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="24" stopIfTrue="1">
+      <formula>$A12="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="26" stopIfTrue="1">
+      <formula>OR($A12="audio", $A12="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
+      <formula>$A12="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="28" stopIfTrue="1">
       <formula>OR($A12="date", $A12="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="29" stopIfTrue="1">
+      <formula>$A12="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="30" stopIfTrue="1">
       <formula>$A12="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="2" stopIfTrue="1">
-      <formula>$A12="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="145" priority="3" stopIfTrue="1">
-      <formula>OR($A12="audio", $A12="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="144" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="31" stopIfTrue="1">
       <formula>OR($A12="geopoint", $A12="geoshape", $A12="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="27" stopIfTrue="1">
-      <formula>$A12="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="142" priority="4" stopIfTrue="1">
-      <formula>$A12="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="141" priority="5" stopIfTrue="1">
-      <formula>OR($A12="date", $A12="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="32" stopIfTrue="1">
       <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="139" priority="6" stopIfTrue="1">
-      <formula>OR($A12="calculate", $A12="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="138" priority="7" stopIfTrue="1">
-      <formula>$A12="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="137" priority="8" stopIfTrue="1">
-      <formula>$A12="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="26" stopIfTrue="1">
-      <formula>OR($A12="audio", $A12="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="24" stopIfTrue="1">
-      <formula>$A12="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="23" stopIfTrue="1">
-      <formula>$A12="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="133" priority="22" stopIfTrue="1">
-      <formula>$A12="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="132" priority="21" stopIfTrue="1">
-      <formula>$A12="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="131" priority="20" stopIfTrue="1">
-      <formula>$A12="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="9" stopIfTrue="1">
-      <formula>OR($A12="geopoint", $A12="geoshape", $A12="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="129" priority="19" stopIfTrue="1">
-      <formula>$A12="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="128" priority="10" stopIfTrue="1">
-      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="127" priority="18" stopIfTrue="1">
-      <formula>$A12="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="11" stopIfTrue="1">
-      <formula>OR($A12="username", $A12="phonenumber", $A12="start", $A12="end", $A12="deviceid", $A12="subscriberid", $A12="simserial", $A12="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="12" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="124" priority="13" stopIfTrue="1">
-      <formula>$A12="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="123" priority="14" stopIfTrue="1">
-      <formula>$A12="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="122" priority="15" stopIfTrue="1">
-      <formula>$A12="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="121" priority="16" stopIfTrue="1">
-      <formula>$A12="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="17" stopIfTrue="1">
-      <formula>$A12="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="1" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D1048576">
-    <cfRule type="expression" dxfId="118" priority="2083" stopIfTrue="1">
-      <formula>$A12="integer"</formula>
+    <cfRule type="expression" dxfId="118" priority="1958" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="117" priority="1960" stopIfTrue="1">
       <formula>$A12="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="1968" stopIfTrue="1">
-      <formula>$A12="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="1967" stopIfTrue="1">
-      <formula>$A12="begin repeat"</formula>
+    <cfRule type="expression" dxfId="116" priority="1962" stopIfTrue="1">
+      <formula>$A12="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="1964" stopIfTrue="1">
+      <formula>$A12="text"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="114" priority="1965" stopIfTrue="1">
       <formula>$A12="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="1964" stopIfTrue="1">
-      <formula>$A12="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="1962" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="1967" stopIfTrue="1">
+      <formula>$A12="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="1968" stopIfTrue="1">
+      <formula>$A12="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="1970" stopIfTrue="1">
+      <formula>$A12="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="2081" stopIfTrue="1">
+      <formula>$A12="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="2083" stopIfTrue="1">
       <formula>$A12="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="2081" stopIfTrue="1">
-      <formula>$A12="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="1970" stopIfTrue="1">
-      <formula>$A12="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="1958" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:E11 E12:E1048576">
-    <cfRule type="expression" dxfId="108" priority="86" stopIfTrue="1">
+  <conditionalFormatting sqref="D1:D11">
+    <cfRule type="expression" dxfId="108" priority="83" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="84" stopIfTrue="1">
+      <formula>$A1="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="85" stopIfTrue="1">
+      <formula>OR($A1="audio", $A1="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="86" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="103" stopIfTrue="1">
-      <formula>$A1="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="87" stopIfTrue="1">
+      <formula>OR($A1="date", $A1="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="88" stopIfTrue="1">
+      <formula>OR($A1="calculate", $A1="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="89" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="90" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="88" stopIfTrue="1">
-      <formula>OR($A1="calculate", $A1="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="91" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="87" stopIfTrue="1">
-      <formula>OR($A1="date", $A1="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="92" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="93" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="104" stopIfTrue="1">
-      <formula>$A1="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="94" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="85" stopIfTrue="1">
-      <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="96" priority="95" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="84" stopIfTrue="1">
-      <formula>$A1="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="96" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="83" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="92" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="97" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="98" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="99" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="100" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="101" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="102" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="88" priority="103" stopIfTrue="1">
+      <formula>$A1="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="104" stopIfTrue="1">
+      <formula>$A1="begin group"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:V1048576 A1:C11">
+  <conditionalFormatting sqref="E1:U1048576 A1:C11">
     <cfRule type="expression" dxfId="86" priority="2132" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 A12:C16 B17:C1048576">
+  <conditionalFormatting sqref="F1:F1048576 A12:C16 B17:C1048576">
     <cfRule type="expression" dxfId="85" priority="1813" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576 A12:C16 B17:C1048576 G1:G1048576">
+  <conditionalFormatting sqref="J1:J1048576 A12:C16 B17:C1048576 F1:F1048576">
     <cfRule type="expression" dxfId="84" priority="1838" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
@@ -6198,14 +6205,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="27" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1" collapsed="1"/>
@@ -6235,14 +6242,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="C2" s="16" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2507151302</v>
+        <v>2509241102</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>358</v>
@@ -10066,11 +10073,11 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5">
-    <cfRule type="expression" dxfId="82" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="95" stopIfTrue="1">
+      <formula>$A5="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="95" stopIfTrue="1">
-      <formula>$A5="begin repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="80" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
@@ -10089,40 +10096,40 @@
     <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
+      <formula>OR($A5="audio audit", $A5="text audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
+      <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
+      <formula>$A5="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
+      <formula>$A5="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+      <formula>$A5="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="92" stopIfTrue="1">
-      <formula>$A5="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="83" stopIfTrue="1">
-      <formula>OR($A5="audio audit", $A5="text audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="90" stopIfTrue="1">
-      <formula>$A5="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="84" stopIfTrue="1">
-      <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="88" stopIfTrue="1">
-      <formula>$A5="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="86" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5">
-    <cfRule type="expression" dxfId="68" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="67" stopIfTrue="1">
+      <formula>$A5="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="69" stopIfTrue="1">
+      <formula>OR($A5="audio", $A5="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="71" stopIfTrue="1">
+      <formula>$A5="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="71" stopIfTrue="1">
-      <formula>$A5="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="69" stopIfTrue="1">
-      <formula>OR($A5="audio", $A5="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="67" stopIfTrue="1">
-      <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
@@ -10146,11 +10153,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="60" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="70" stopIfTrue="1">
+      <formula>$A5="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="70" stopIfTrue="1">
-      <formula>$A5="image"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="58" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
@@ -10189,86 +10196,86 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="49" priority="41" stopIfTrue="1">
-      <formula>OR($A5="date", $A5="datetime")</formula>
+    <cfRule type="expression" dxfId="49" priority="39" stopIfTrue="1">
+      <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="48" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
-      <formula>$A5="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="45" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="39" stopIfTrue="1">
-      <formula>OR($A5="audio", $A5="video")</formula>
+    <cfRule type="expression" dxfId="47" priority="41" stopIfTrue="1">
+      <formula>OR($A5="date", $A5="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="42" stopIfTrue="1">
+      <formula>$A5="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="43" stopIfTrue="1">
+      <formula>$A5="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="44" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
-      <formula>$A5="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="42" stopIfTrue="1">
-      <formula>$A5="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="45" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="47" stopIfTrue="1">
+      <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
     <cfRule type="expression" dxfId="40" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="32" stopIfTrue="1">
+      <formula>$A5="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="36" stopIfTrue="1">
+      <formula>$A5="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="37" stopIfTrue="1">
+      <formula>$A5="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="37" stopIfTrue="1">
-      <formula>$A5="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="36" stopIfTrue="1">
-      <formula>$A5="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="32" stopIfTrue="1">
-      <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:O5">
     <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="35" stopIfTrue="1">
-      <formula>$A5="end repeat"</formula>
+    <cfRule type="expression" dxfId="34" priority="33" stopIfTrue="1">
+      <formula>$A5="integer"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="33" stopIfTrue="1">
-      <formula>$A5="integer"</formula>
+    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
+      <formula>$A5="end repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:P5">
-    <cfRule type="expression" dxfId="31" priority="11" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="10" stopIfTrue="1">
-      <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
-      <formula>OR($A5="audio audit", $A5="text audit")</formula>
+    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
+      <formula>OR($A5="calculate", $A5="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="6" stopIfTrue="1">
+      <formula>$A5="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
+      <formula>$A5="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="7" stopIfTrue="1">
-      <formula>$A5="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="6" stopIfTrue="1">
-      <formula>$A5="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
-      <formula>OR($A5="calculate", $A5="calculate_here")</formula>
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
+      <formula>OR($A5="audio audit", $A5="text audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
+      <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:AD5">
@@ -10286,46 +10293,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="20" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="12" stopIfTrue="1">
+      <formula>$A5="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="13" stopIfTrue="1">
+      <formula>$A5="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="14" stopIfTrue="1">
+      <formula>$A5="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="15" stopIfTrue="1">
+      <formula>$A5="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
+      <formula>$A5="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+      <formula>$A5="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="12" stopIfTrue="1">
-      <formula>$A5="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="13" stopIfTrue="1">
-      <formula>$A5="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
-      <formula>$A5="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
-      <formula>$A5="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
-      <formula>$A5="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
-      <formula>$A5="end group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:AD5">
-    <cfRule type="expression" dxfId="13" priority="65" stopIfTrue="1">
-      <formula>$A5="begin group"</formula>
+    <cfRule type="expression" dxfId="13" priority="52" stopIfTrue="1">
+      <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="52" stopIfTrue="1">
-      <formula>OR($A5="calculate", $A5="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="57" stopIfTrue="1">
+      <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
@@ -10348,8 +10355,8 @@
     <cfRule type="expression" dxfId="1" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="57" stopIfTrue="1">
-      <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
+    <cfRule type="expression" dxfId="0" priority="65" stopIfTrue="1">
+      <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>